<commit_message>
unpopulated data for vis updated
</commit_message>
<xml_diff>
--- a/2_Vis/Copy of -- TRG - Projected Occupancy and Costs.xlsx
+++ b/2_Vis/Copy of -- TRG - Projected Occupancy and Costs.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="21840" windowHeight="12855"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="25120" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>ONS.LA.Code</t>
   </si>
@@ -54,18 +59,6 @@
     <t>Projected.Population.85pl</t>
   </si>
   <si>
-    <t>LA.Funded.Occupancy.18-64</t>
-  </si>
-  <si>
-    <t>LA.Funded.Occupancy.65-74</t>
-  </si>
-  <si>
-    <t>LA.Funded.Occupancy.75-84</t>
-  </si>
-  <si>
-    <t>LA.Funded.Occupancy.85pl</t>
-  </si>
-  <si>
     <t>Total.Beds</t>
   </si>
   <si>
@@ -87,9 +80,6 @@
     <t>Other Supplementary LA Cost Metrics</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>..</t>
   </si>
   <si>
@@ -102,9 +92,6 @@
     <t>LA.Cost.Of.Care.75-84</t>
   </si>
   <si>
-    <t>LA.Cost.Of.Care.75pl</t>
-  </si>
-  <si>
     <t>Estiamted LA-funded occupancy, x LA Avg Gross Weekly Cost of Care</t>
   </si>
   <si>
@@ -118,16 +105,84 @@
   </si>
   <si>
     <t>From ONS SRC dataset</t>
+  </si>
+  <si>
+    <t>Projection for that year</t>
+  </si>
+  <si>
+    <t>Projectin for that year</t>
+  </si>
+  <si>
+    <t>LA.Funded.Occupancy.18-64_Resi</t>
+  </si>
+  <si>
+    <t>LA.Funded.Occupancy.18-64_Nursing</t>
+  </si>
+  <si>
+    <t>Talk to shyam</t>
+  </si>
+  <si>
+    <t>Total number of people</t>
+  </si>
+  <si>
+    <t>Use for ratio between 2015 and projected population</t>
+  </si>
+  <si>
+    <t>total number of beds projected by population increase</t>
+  </si>
+  <si>
+    <t>sum of the other columns</t>
+  </si>
+  <si>
+    <t>LA.Cost.Of.Care.85pl</t>
+  </si>
+  <si>
+    <t>LA.Funded.Occupancy.65-74_Resi</t>
+  </si>
+  <si>
+    <t>LA.Funded.Occupancy.65-74_Nursing</t>
+  </si>
+  <si>
+    <t>LA.Funded.Occupancy.75-84_Resi</t>
+  </si>
+  <si>
+    <t>LA.Funded.Occupancy.75-84_Nursing</t>
+  </si>
+  <si>
+    <t>LA.Funded.Occupancy.85pl_Resi</t>
+  </si>
+  <si>
+    <t>LA.Funded.Occupancy.85pl_Nursing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -149,13 +204,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -398,32 +474,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="34" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="24" width="21.28515625" customWidth="1"/>
-    <col min="25" max="25" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="34" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34" customWidth="1"/>
+    <col min="18" max="18" width="34" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="34" customWidth="1"/>
+    <col min="20" max="20" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="21.33203125" customWidth="1"/>
+    <col min="29" max="29" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -464,139 +548,181 @@
         <v>11</v>
       </c>
       <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="AE1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="C2">
+        <v>2015</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
+        <v>29</v>
+      </c>
+      <c r="V2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
+      <c r="T3" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="V3" t="s">
+        <v>16</v>
+      </c>
+      <c r="W3" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+    </row>
+    <row r="4" spans="1:33">
+      <c r="V4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+    </row>
+    <row r="5" spans="1:33">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="V1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="F5" t="s">
         <v>27</v>
       </c>
-      <c r="X1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y5" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="N3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>19</v>
-      </c>
-      <c r="R3" t="s">
-        <v>20</v>
-      </c>
-      <c r="S3" t="s">
-        <v>20</v>
-      </c>
-      <c r="T3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U3" t="s">
-        <v>19</v>
-      </c>
-      <c r="V3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W3" t="s">
-        <v>19</v>
-      </c>
-      <c r="X3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U5" t="s">
-        <v>29</v>
-      </c>
-      <c r="V5" t="s">
-        <v>29</v>
-      </c>
-      <c r="W5" t="s">
-        <v>29</v>
-      </c>
-      <c r="X5" t="s">
-        <v>29</v>
-      </c>
+      <c r="Z5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -606,9 +732,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -618,8 +749,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Copy of -- TRG - Projected Occupancy and Costs.xlsx updated
</commit_message>
<xml_diff>
--- a/2_Vis/Copy of -- TRG - Projected Occupancy and Costs.xlsx
+++ b/2_Vis/Copy of -- TRG - Projected Occupancy and Costs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="25120" windowHeight="15520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -477,7 +477,7 @@
   <dimension ref="A1:AG5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>